<commit_message>
Update Bill Of Materials_final.xlsx
</commit_message>
<xml_diff>
--- a/Bill Of Materials_final.xlsx
+++ b/Bill Of Materials_final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My_files\Study\Github\ECE-411-Group-10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4BCA7C4E-8596-4BD1-978E-1208F27E30FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8218D1B0-B87D-4C92-8E59-A18AD3F29098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6975" yWindow="5595" windowWidth="28125" windowHeight="15570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6840" yWindow="4695" windowWidth="28125" windowHeight="15570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -758,7 +758,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -932,7 +932,7 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="2">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>39</v>
@@ -959,13 +959,13 @@
         <v>0.2</v>
       </c>
       <c r="J9" s="13">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="2">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>40</v>
@@ -992,13 +992,13 @@
         <v>0.2</v>
       </c>
       <c r="J10" s="13">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="2">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>41</v>
@@ -1025,13 +1025,13 @@
         <v>0.2</v>
       </c>
       <c r="J11" s="13">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="K11" s="2"/>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="2">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>42</v>
@@ -1058,7 +1058,7 @@
         <v>0.2</v>
       </c>
       <c r="J12" s="13">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="K12" s="2"/>
     </row>
@@ -1266,7 +1266,7 @@
       </c>
       <c r="J19" s="12">
         <f>SUM(J7:J18)</f>
-        <v>36.870000000000005</v>
+        <v>29.669999999999998</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.75" thickBot="1">

</xml_diff>